<commit_message>
almost TA and sales page done
</commit_message>
<xml_diff>
--- a/sample_csv/ta.xlsx
+++ b/sample_csv/ta.xlsx
@@ -488,8 +488,8 @@
   </sheetPr>
   <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AF1" activeCellId="0" sqref="AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -510,10 +510,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="10.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="9.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
all bug fixed in sales, VM, TA
</commit_message>
<xml_diff>
--- a/sample_csv/ta.xlsx
+++ b/sample_csv/ta.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="77">
   <si>
     <t xml:space="preserve">SL.No</t>
   </si>
@@ -123,6 +123,9 @@
     <t xml:space="preserve">Resume</t>
   </si>
   <si>
+    <t xml:space="preserve">Remarks</t>
+  </si>
+  <si>
     <t xml:space="preserve">Archived</t>
   </si>
   <si>
@@ -159,10 +162,7 @@
     <t xml:space="preserve">New Comment 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Hi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yo</t>
+    <t xml:space="preserve">Sunil</t>
   </si>
   <si>
     <t xml:space="preserve">Naukri-MM</t>
@@ -183,6 +183,9 @@
     <t xml:space="preserve">resume1</t>
   </si>
   <si>
+    <t xml:space="preserve">Developer</t>
+  </si>
+  <si>
     <t xml:space="preserve">Closed</t>
   </si>
   <si>
@@ -207,10 +210,7 @@
     <t xml:space="preserve">New Comment 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Hello</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hello</t>
+    <t xml:space="preserve">Pankaj</t>
   </si>
   <si>
     <t xml:space="preserve">one t1</t>
@@ -225,6 +225,9 @@
     <t xml:space="preserve">resume2</t>
   </si>
   <si>
+    <t xml:space="preserve">Tester</t>
+  </si>
+  <si>
     <t xml:space="preserve">Manju</t>
   </si>
   <si>
@@ -240,7 +243,7 @@
     <t xml:space="preserve">New Comment 3</t>
   </si>
   <si>
-    <t xml:space="preserve">good morning</t>
+    <t xml:space="preserve">venkatesh</t>
   </si>
   <si>
     <t xml:space="preserve">two t1</t>
@@ -486,10 +489,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG4"/>
+  <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AF1" activeCellId="0" sqref="AF1"/>
+      <selection pane="topLeft" activeCell="AH4" activeCellId="0" sqref="AH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -613,31 +616,34 @@
       <c r="AG1" s="0" t="s">
         <v>32</v>
       </c>
+      <c r="AH1" s="0" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>45089</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I2" s="3" t="n">
         <v>9</v>
@@ -646,7 +652,7 @@
         <v>4.6</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="L2" s="3" t="n">
         <v>8</v>
@@ -661,34 +667,34 @@
         <v>0</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R2" s="3" t="n">
         <v>9962740967</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="X2" s="4" t="n">
         <v>45089</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="Z2" s="4" t="n">
         <v>45089</v>
@@ -713,6 +719,9 @@
       </c>
       <c r="AG2" s="0" t="s">
         <v>52</v>
+      </c>
+      <c r="AH2" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -720,25 +729,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>45089</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I3" s="3" t="n">
         <v>3.8</v>
@@ -747,7 +756,7 @@
         <v>3.8</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L3" s="3" t="n">
         <v>4</v>
@@ -762,34 +771,34 @@
         <v>9</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R3" s="3" t="n">
         <v>9727265510</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="X3" s="4" t="n">
         <v>45089</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="Z3" s="4" t="n">
         <v>45089</v>
@@ -814,6 +823,9 @@
       </c>
       <c r="AG3" s="0" t="s">
         <v>66</v>
+      </c>
+      <c r="AH3" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -821,25 +833,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>45096</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I4" s="3" t="n">
         <v>5</v>
@@ -848,7 +860,7 @@
         <v>4</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L4" s="3" t="n">
         <v>2</v>
@@ -863,34 +875,34 @@
         <v>45</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R4" s="3" t="n">
         <v>9916511663</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="X4" s="4" t="n">
         <v>45096</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="Z4" s="4" t="n">
         <v>45096</v>
@@ -905,16 +917,19 @@
         <v>49</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AF4" s="0" t="s">
         <v>48</v>
       </c>
       <c r="AG4" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+      <c r="AH4" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>